<commit_message>
Added data from trial 22
and confirmed data for other runs
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_PB-constant_summary.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_PB-constant_summary.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\Travel-Conferences\BOSC_ISMB_2025\21 original runs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560CC8FF-CE0B-4524-9718-0931674BB25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="845" xr2:uid="{61DF7949-D53D-4105-9735-EE06691314FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="845"/>
   </bookViews>
   <sheets>
     <sheet name="Pb Constant" sheetId="1" r:id="rId1"/>
@@ -35,29 +29,14 @@
     <sheet name="19" sheetId="6" r:id="rId20"/>
     <sheet name="20" sheetId="5" r:id="rId21"/>
     <sheet name="21" sheetId="4" r:id="rId22"/>
+    <sheet name="22" sheetId="26" r:id="rId23"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="8">
   <si>
     <t>Trial</t>
   </si>
@@ -86,8 +65,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,24 +127,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{70519227-5B63-4686-ADE9-D4CF5CB72DF2}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{6D324F20-C91C-4E45-A4F0-8B5D47920066}"/>
-    <cellStyle name="Normal 4" xfId="1" xr:uid="{530E491E-9E52-4105-A481-D94D8643FA3F}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="4"/>
+    <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -173,15 +156,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -220,6 +200,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -228,26 +209,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -320,34 +281,34 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -392,39 +353,39 @@
                   <c:v>6.4617949121827165E-10</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>7.9427480426631953E-10</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1.2759981366433912E-9</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3.409843017575834E-9</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>8.4351201529012733E-9</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2.3977996253966481E-8</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>3.1537391407770736E-3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>3.7478482197808591</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>4.4999161461543888</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>4.500108444748113</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>7.4670175960146183</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.9870957021480429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3AE6-4C22-9488-42930035D488}"/>
             </c:ext>
@@ -440,11 +401,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1279891743"/>
-        <c:axId val="1279897503"/>
+        <c:axId val="52838400"/>
+        <c:axId val="52708480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1279891743"/>
+        <c:axId val="52838400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1279897503"/>
+        <c:crossAx val="52708480"/>
         <c:crossesAt val="1.0000000000000007E-13"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -495,7 +456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1279897503"/>
+        <c:axId val="52708480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -549,7 +510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1279891743"/>
+        <c:crossAx val="52838400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -563,14 +524,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1168,7 +1129,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1498,27 +1459,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7478D67-BA7D-48FA-92AF-8000621A116E}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -1547,7 +1508,7 @@
         <v>9.9870957021480429</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="1">
         <v>15</v>
       </c>
@@ -1562,7 +1523,7 @@
         <v>3.7478482197808591</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="1">
         <v>19</v>
       </c>
@@ -1577,7 +1538,7 @@
         <v>8.4351201529012733E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -1592,7 +1553,7 @@
         <v>2.3977996253966481E-8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1607,7 +1568,7 @@
         <v>4.3225020136638796E-11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="1">
         <v>9</v>
       </c>
@@ -1622,7 +1583,7 @@
         <v>4.2707826655854999E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -1637,7 +1598,7 @@
         <v>2.6853689225398418E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1652,7 +1613,7 @@
         <v>3.9195619734684774E-11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1667,7 +1628,7 @@
         <v>6.2412407158026194E-11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -1682,7 +1643,7 @@
         <v>1.6926656966503639E-12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="1">
         <v>13</v>
       </c>
@@ -1697,177 +1658,192 @@
         <v>3.1537391407770736E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="1">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <f>'22'!B16</f>
+        <v>7.9427480426631953E-10</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>4.9336643405195255E-10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="1">
         <v>20</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <f>'20'!B16</f>
         <v>1.2759981366433912E-9</v>
       </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>4.9336643405195255E-10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>6.4617949121827165E-10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="1">
         <v>21</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <f>'21'!B16</f>
         <v>3.409843017575834E-9</v>
       </c>
-      <c r="D14">
-        <v>13</v>
-      </c>
-      <c r="E14">
-        <v>6.4617949121827165E-10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>4.500108444748113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <f>'3'!B16</f>
         <v>8.4351201529012733E-9</v>
       </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
-      <c r="E15">
-        <v>4.500108444748113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>8.444515206463839E-12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15">
+      <c r="A17" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <f>'4'!B16</f>
         <v>2.3977996253966481E-8</v>
       </c>
-      <c r="D16">
-        <v>15</v>
-      </c>
-      <c r="E16">
-        <v>8.444515206463839E-12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>1.3404323801768158E-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15">
+      <c r="A18" s="1">
         <v>11</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <f>'11'!B16</f>
         <v>3.1537391407770736E-3</v>
       </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-      <c r="E17">
-        <v>1.3404323801768158E-10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>4.4999161461543888</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15">
+      <c r="A19" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <f>'2'!B16</f>
         <v>3.7478482197808591</v>
       </c>
-      <c r="D18">
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>7.4670175960146183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15">
+      <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="E18">
-        <v>4.4999161461543888</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <f>'17'!B16</f>
         <v>4.4999161461543888</v>
       </c>
-      <c r="D19">
-        <v>18</v>
-      </c>
-      <c r="E19">
-        <v>7.4670175960146183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>1.3414616072216297E-11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15">
+      <c r="A21" s="1">
         <v>14</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <f>'14'!B16</f>
         <v>4.500108444748113</v>
       </c>
-      <c r="D20">
-        <v>19</v>
-      </c>
-      <c r="E20">
-        <v>1.3414616072216297E-11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>1.2759981366433912E-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15">
+      <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <f>'18'!B16</f>
         <v>7.4670175960146183</v>
       </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
-      <c r="E21">
-        <v>1.2759981366433912E-9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>3.409843017575834E-9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <f>'1'!B16</f>
         <v>9.9870957021480429</v>
       </c>
-      <c r="D22">
-        <v>21</v>
-      </c>
-      <c r="E22">
-        <v>3.409843017575834E-9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1">
+        <v>7.9427480426631953E-10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15">
+      <c r="D24" t="s">
         <v>2</v>
       </c>
-      <c r="E23">
-        <f>AVERAGE(E2:E22)</f>
-        <v>1.4383399946296831</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="E24">
+        <f>AVERAGE(E2:E23)</f>
+        <v>1.3729609040008008</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15">
+      <c r="D25" t="s">
         <v>3</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <f>SUM(E2:E23)</f>
-        <v>31.643479881853029</v>
+        <v>30.205139888017619</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E25">
-    <sortCondition ref="D2:D25"/>
+  <sortState ref="A2:B23">
+    <sortCondition ref="B2:B23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1875,16 +1851,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83615C64-E794-4FBF-9071-AD2A44D1D0A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1898,7 +1874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1912,7 +1888,7 @@
         <v>0.9999924689630838</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1902,7 @@
         <v>1.9999998684867899</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1954,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1968,7 +1944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1982,7 +1958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1996,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2010,7 +1986,7 @@
         <v>5.6716517033127845E-11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2024,7 +2000,7 @@
         <v>1.7295724430768326E-14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -2038,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>6.2412407158026194E-11</v>
@@ -2050,16 +2026,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40157B9F-6434-4685-B5EC-1BE86917077B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2073,7 +2049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2087,7 +2063,7 @@
         <v>1.0000008175527222</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2101,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2115,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2129,7 +2105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2143,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2157,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2185,7 +2161,7 @@
         <v>6.6839245355642401E-13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>3.2133244125492189E-16</v>
@@ -2199,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>1.0067296043592571E-14</v>
@@ -2213,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.6926656966503639E-12</v>
@@ -2225,16 +2201,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA995C32-351D-49BE-93C9-576C97468297}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2248,7 +2224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2262,7 +2238,7 @@
         <v>-1.0172272597706966</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2276,7 +2252,7 @@
         <v>1.9999995297975863</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2290,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2304,7 +2280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2318,7 +2294,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2332,7 +2308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2346,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>2.7397305636002898E-3</v>
@@ -2360,7 +2336,7 @@
         <v>2.9677847920706187E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2374,7 +2350,7 @@
         <v>2.2109030982257223E-13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2388,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.1537391407770736E-3</v>
@@ -2400,16 +2376,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EF0B3D-B400-4975-8CA7-B989EBF30B53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2423,7 +2399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2437,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2451,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2465,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2479,7 +2455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2493,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2507,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2521,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2535,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>2.0931521124755023E-10</v>
@@ -2549,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>1.3998208124324171E-10</v>
@@ -2563,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.9336643405195255E-10</v>
@@ -2575,16 +2551,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8DD21A-91B9-413D-87A7-237727AE6C19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2598,7 +2574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2612,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2626,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2640,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2654,7 +2630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2668,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2682,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2696,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.2117972774883117E-14</v>
@@ -2710,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2724,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>4.9231416426641019E-10</v>
@@ -2738,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>6.4617949121827165E-10</v>
@@ -2750,16 +2726,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142147BB-8850-42AC-BF7C-800B472E78BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2773,7 +2749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2787,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2801,7 +2777,7 @@
         <v>1.9999991219977338</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2815,7 +2791,7 @@
         <v>-0.50001800316934852</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2829,7 +2805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2843,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2857,7 +2833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2871,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.2544997651263904E-14</v>
@@ -2885,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2899,7 +2875,7 @@
         <v>7.7088797949570512E-13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2500544349151697</v>
@@ -2913,7 +2889,7 @@
         <v>2.25005400983216</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.500108444748113</v>
@@ -2925,16 +2901,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E82B8F-29E1-4315-852A-14C5AE3CB1A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2948,7 +2924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2962,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2976,7 +2952,7 @@
         <v>1.9999990033771018</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2990,7 +2966,7 @@
         <v>0.999997303411302</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3004,7 +2980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3018,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3032,7 +3008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3046,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3060,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3074,7 +3050,7 @@
         <v>9.9325720123319841E-13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3088,7 +3064,7 @@
         <v>7.2715906062001469E-12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>8.444515206463839E-12</v>
@@ -3100,16 +3076,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134DEB53-E5AB-4274-AFB9-D4C08DD6EBEC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3123,7 +3099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3137,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3151,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3165,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3179,7 +3155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3193,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3207,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3221,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3235,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3249,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>6.3755491215956899E-11</v>
@@ -3263,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.3404323801768158E-10</v>
@@ -3275,16 +3251,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F142013-565D-4117-8E1E-C10958E38EE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3298,7 +3274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3312,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3326,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3340,7 +3316,7 @@
         <v>-0.49998599303701374</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3354,7 +3330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3368,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3382,7 +3358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3396,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>3.3757069090043225E-14</v>
@@ -3410,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>8.2639920641830585E-13</v>
@@ -3424,7 +3400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2499581668462927</v>
@@ -3438,7 +3414,7 @@
         <v>2.249957979307236</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.4999161461543888</v>
@@ -3450,16 +3426,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01013357-7328-4AD5-90E3-3258776CEF5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3473,7 +3449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3487,7 +3463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3501,7 +3477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3515,7 +3491,7 @@
         <v>-0.1155248415218823</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3529,7 +3505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3543,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3557,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3571,7 +3547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3585,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3599,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>4.9779558368610894</v>
@@ -3613,13 +3589,13 @@
         <v>1.2443956720524207</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>7.4670175960146183</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="4"/>
     </row>
   </sheetData>
@@ -3628,16 +3604,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B97CF0-99B2-4337-A953-1577F71FE002}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3651,7 +3627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3665,7 +3641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3679,7 +3655,7 @@
         <v>2.2730106450422567E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3693,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3707,7 +3683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3721,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3735,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3749,7 +3725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3763,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0.95505641979740763</v>
@@ -3777,7 +3753,7 @@
         <v>0.95505644483840235</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>4.0384914627053421</v>
@@ -3791,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>9.9870957021480429</v>
@@ -3803,16 +3779,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EDBDA-A255-485C-A114-9E4EBC1235F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3826,7 +3802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3840,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3854,7 +3830,7 @@
         <v>1.9999979743631551</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3868,7 +3844,7 @@
         <v>0.99999999490349967</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3882,7 +3858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3896,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3910,7 +3886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3924,7 +3900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>9.1908694083278319E-12</v>
@@ -3938,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3952,7 +3928,7 @@
         <v>4.1032046275247458E-12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3966,7 +3942,7 @@
         <v>2.5974315642928312E-17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.3414616072216297E-11</v>
@@ -3978,16 +3954,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300E425B-5620-4431-B514-B1BBE2549DEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4001,7 +3977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4015,7 +3991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4029,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4043,7 +4019,7 @@
         <v>1.0000068267736866</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4057,7 +4033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4071,7 +4047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4085,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4099,7 +4075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4113,7 +4089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>8.6366800982543046E-10</v>
@@ -4127,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4141,7 +4117,7 @@
         <v>4.6604838967707122E-11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.2759981366433912E-9</v>
@@ -4153,16 +4129,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F7287-090A-46B7-BA3C-27A59C785353}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4176,7 +4152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4190,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4204,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4218,7 +4194,7 @@
         <v>0.99999744015291026</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4232,7 +4208,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4246,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4260,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4274,7 +4250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4288,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>2.411419337246953E-9</v>
@@ -4302,7 +4278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>1.1778647682694007E-12</v>
@@ -4316,7 +4292,7 @@
         <v>6.5528171228747746E-12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.409843017575834E-9</v>
@@ -4327,17 +4303,193 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0089BC1C-C5EA-49A9-99C3-DFC372691FF0}">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>-1.0000105817500466</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>-1.9999939572578724</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.9999745957968253</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.0000006427276698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12">
+        <f>(B8-B2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="0">(C8-C2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="B13">
+        <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
+        <v>1.1197343404968015E-10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>3.6514732420254871E-11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>6.4537353893891842E-10</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>4.1309885746603065E-13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="B16" s="2">
+        <f>SUM(B12:D14)</f>
+        <v>7.9427480426631953E-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4351,7 +4503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4365,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4379,7 +4531,7 @@
         <v>0.20959841482607589</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4393,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4407,7 +4559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4421,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4435,7 +4587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4449,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4463,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>2.4986502459103144</v>
@@ -4477,7 +4629,7 @@
         <v>0.62473466584545201</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -4491,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.7478482197808591</v>
@@ -4503,16 +4655,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313B83BB-D4F2-401B-BF0B-10D69BB3D6FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4526,7 +4678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4540,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4554,7 +4706,7 @@
         <v>1.0000029979972769</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4568,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4582,7 +4734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4596,7 +4748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4610,7 +4762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4624,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>3.2307628006243284E-9</v>
@@ -4638,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -4652,7 +4804,7 @@
         <v>8.9879876721605509E-12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>1.0338593764804853E-13</v>
@@ -4666,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>8.4351201529012733E-9</v>
@@ -4678,16 +4830,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3D4390-3995-460B-ABEF-C18D95517F47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4701,7 +4853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4715,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4729,7 +4881,7 @@
         <v>0.99991215307687364</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4743,7 +4895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4757,7 +4909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4771,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4785,7 +4937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4799,7 +4951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4813,7 +4965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -4827,7 +4979,7 @@
         <v>7.7170819027678425E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -4841,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.3977996253966481E-8</v>
@@ -4853,16 +5005,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB9E05B-3793-41C3-B94B-40F5229BD806}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4876,7 +5028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4890,7 +5042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4904,7 +5056,7 @@
         <v>1.0000004213127522</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4918,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4932,7 +5084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4946,7 +5098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4960,7 +5112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4974,7 +5126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>9.8086104354683515E-12</v>
@@ -4988,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5002,7 +5154,7 @@
         <v>1.7750443520107228E-13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5016,7 +5168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.3225020136638796E-11</v>
@@ -5028,16 +5180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6FF64C-47D1-4ACB-8BCD-8DB8DA890DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5051,7 +5203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5065,7 +5217,7 @@
         <v>-0.99998063737965859</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5079,7 +5231,7 @@
         <v>1.9999988103281454</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5093,7 +5245,7 @@
         <v>-1.9999994966945129</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5107,7 +5259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5121,7 +5273,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5135,7 +5287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5149,7 +5301,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5163,7 +5315,7 @@
         <v>3.7491106648566631E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5177,7 +5329,7 @@
         <v>1.4153191215905655E-12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5191,7 +5343,7 @@
         <v>2.533164133098576E-13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.2707826655854999E-10</v>
@@ -5203,16 +5355,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C51A42-0714-4274-9CCE-FD3E5D511EAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -5226,7 +5378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5240,7 +5392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -5254,7 +5406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -5268,7 +5420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -5282,7 +5434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -5296,7 +5448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -5310,7 +5462,7 @@
         <v>0.99999410832973146</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -5324,7 +5476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.1632944952080548E-14</v>
@@ -5338,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>2.2815686498951899E-10</v>
@@ -5352,7 +5504,7 @@
         <v>3.4711778553233323E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5366,7 +5518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.6853689225398418E-10</v>
@@ -5378,16 +5530,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743B6CCE-E37A-4B9D-B598-F019BFB3039F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5401,7 +5553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5415,7 +5567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5429,7 +5581,7 @@
         <v>0.99999834970933899</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5443,7 +5595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5457,7 +5609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5471,7 +5623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5485,7 +5637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5499,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5513,7 +5665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5527,7 +5679,7 @@
         <v>2.7234592658332056E-12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>8.7361186669632664E-12</v>
@@ -5541,7 +5693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.9195619734684774E-11</v>
@@ -5553,12 +5705,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5757,17 +5908,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7bf50b4b-6300-445a-aea1-306a2291592c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5792,11 +5953,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>